<commit_message>
fix: switch project by changing config file
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub.xlsx
@@ -399,13 +399,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>24.02.2023</v>
+        <v>27.02.2023</v>
       </c>
       <c r="C2" t="str">
-        <v>https://github.com/tibonto/dr/commit/08cc171ae8fe31f2c84c826b4cc42f722158e303</v>
+        <v>https://github.com/ifx-dr/Update-Test-DR-Sub-Onto/commit/ac9aef219f062221dc147d65b4fdfc5e5930804d</v>
       </c>
       <c r="D2" t="str">
-        <v>67db27a29ac4e25c80e0acb9e467a31192d02b45ea812b6b181335d6e138f300</v>
+        <v>fe92b17025819ba09605f801eef9cbea87e7411c9676b28bfb59e5e277132ee6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>